<commit_message>
Air France script done
</commit_message>
<xml_diff>
--- a/AirFranceCargo/Test.xlsx
+++ b/AirFranceCargo/Test.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="13">
   <si>
     <t>WONumber</t>
   </si>
@@ -35,34 +35,34 @@
     <t>Waybill Number</t>
   </si>
   <si>
-    <t>057-81913860</t>
-  </si>
-  <si>
-    <t>057-82664330</t>
-  </si>
-  <si>
-    <t>057-83419685</t>
-  </si>
-  <si>
-    <t>T10115822</t>
-  </si>
-  <si>
-    <t>057-82321831</t>
-  </si>
-  <si>
-    <t>21A0401733</t>
-  </si>
-  <si>
-    <t>057-82321816</t>
-  </si>
-  <si>
-    <t>21A0401268</t>
-  </si>
-  <si>
-    <t>057-82321820</t>
-  </si>
-  <si>
-    <t>21A0401740</t>
+    <t>057-82511516</t>
+  </si>
+  <si>
+    <t>057-19009594</t>
+  </si>
+  <si>
+    <t>057-83699442</t>
+  </si>
+  <si>
+    <t>057-83699453</t>
+  </si>
+  <si>
+    <t>057-96206751</t>
+  </si>
+  <si>
+    <t>24S0041891</t>
+  </si>
+  <si>
+    <t>057-83419232</t>
+  </si>
+  <si>
+    <t>21A0406836</t>
+  </si>
+  <si>
+    <t>057-70312594</t>
+  </si>
+  <si>
+    <t>DJMKEA4230073</t>
   </si>
 </sst>
 </file>
@@ -381,10 +381,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:C7"/>
+      <selection activeCell="A2" sqref="A2:C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -410,10 +410,10 @@
         <v>3</v>
       </c>
       <c r="B2" s="1">
-        <v>2711767899</v>
+        <v>2120668841</v>
       </c>
       <c r="C2" s="1">
-        <v>2711767899</v>
+        <v>2120668841</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -421,54 +421,98 @@
         <v>4</v>
       </c>
       <c r="B3">
-        <v>2812096175</v>
+        <v>2061841172</v>
       </c>
       <c r="C3">
-        <v>2812096175</v>
+        <v>2061841172</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
-      <c r="B4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" t="s">
-        <v>6</v>
+      <c r="B4">
+        <v>2550335038</v>
+      </c>
+      <c r="C4">
+        <v>2550335038</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" t="s">
-        <v>8</v>
+        <v>6</v>
+      </c>
+      <c r="B5">
+        <v>2550334549</v>
+      </c>
+      <c r="C5">
+        <v>2550334549</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" t="s">
-        <v>10</v>
+        <v>6</v>
+      </c>
+      <c r="B6">
+        <v>2550334546</v>
+      </c>
+      <c r="C6">
+        <v>2550334546</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>2550335047</v>
+      </c>
+      <c r="C7">
+        <v>2550335047</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8">
+        <v>2120668847</v>
+      </c>
+      <c r="C8">
+        <v>2120668847</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>11</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B11" t="s">
         <v>12</v>
       </c>
-      <c r="C7" t="s">
-        <v>12</v>
+      <c r="C11">
+        <v>222323293</v>
       </c>
     </row>
   </sheetData>

</xml_diff>